<commit_message>
Update results spreadsheet with new evaluation metrics
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="18">
   <si>
     <t>Pointsoup-SA</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>First seen</t>
+  </si>
+  <si>
+    <t>Kitti</t>
   </si>
   <si>
     <t>Pointsoup-examples</t>
@@ -240,19 +243,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF1F2326"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF1F2326"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF1F2326"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color rgb="FF1F2326"/>
@@ -263,6 +253,19 @@
       <bottom style="thin">
         <color rgb="FF1F2326"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF1F2326"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF1F2326"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF1F2326"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -337,13 +340,13 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -655,56 +658,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" customWidth="1"/>
-    <col min="12" max="12" width="16" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" customWidth="1"/>
-    <col min="23" max="23" width="10.85546875" customWidth="1"/>
-    <col min="24" max="24" width="10.85546875" customWidth="1"/>
-    <col min="25" max="25" width="10.85546875" customWidth="1"/>
-    <col min="26" max="26" width="10.85546875" customWidth="1"/>
-    <col min="27" max="27" width="10.85546875" customWidth="1"/>
-    <col min="28" max="28" width="10.85546875" customWidth="1"/>
-    <col min="29" max="29" width="10.85546875" customWidth="1"/>
-    <col min="30" max="30" width="10.85546875" customWidth="1"/>
-    <col min="31" max="31" width="10.85546875" customWidth="1"/>
-    <col min="32" max="32" width="10.85546875" customWidth="1"/>
-    <col min="33" max="33" width="10.85546875" customWidth="1"/>
-    <col min="34" max="34" width="10.85546875" customWidth="1"/>
-    <col min="35" max="35" width="10.85546875" customWidth="1"/>
-    <col min="36" max="36" width="10.85546875" customWidth="1"/>
-    <col min="37" max="37" width="10.85546875" customWidth="1"/>
-    <col min="38" max="38" width="10.85546875" customWidth="1"/>
-    <col min="39" max="39" width="10.85546875" customWidth="1"/>
-    <col min="40" max="40" width="10.85546875" customWidth="1"/>
-    <col min="41" max="41" width="10.85546875" customWidth="1"/>
-    <col min="42" max="42" width="10.85546875" customWidth="1"/>
-    <col min="43" max="43" width="10.85546875" customWidth="1"/>
-    <col min="44" max="44" width="10.85546875" customWidth="1"/>
-    <col min="45" max="45" width="10.85546875" customWidth="1"/>
-    <col min="46" max="46" width="10.85546875" customWidth="1"/>
-    <col min="47" max="47" width="10.85546875" customWidth="1"/>
-    <col min="48" max="48" width="10.85546875" customWidth="1"/>
-    <col min="49" max="49" width="10.85546875" customWidth="1"/>
-    <col min="50" max="50" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" customWidth="1"/>
+    <col min="23" max="23" width="10.7109375" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" customWidth="1"/>
+    <col min="27" max="27" width="10.7109375" customWidth="1"/>
+    <col min="28" max="28" width="10.7109375" customWidth="1"/>
+    <col min="29" max="29" width="10.7109375" customWidth="1"/>
+    <col min="30" max="30" width="10.7109375" customWidth="1"/>
+    <col min="31" max="31" width="10.7109375" customWidth="1"/>
+    <col min="32" max="32" width="10.7109375" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" customWidth="1"/>
+    <col min="34" max="34" width="10.7109375" customWidth="1"/>
+    <col min="35" max="35" width="10.7109375" customWidth="1"/>
+    <col min="36" max="36" width="10.7109375" customWidth="1"/>
+    <col min="37" max="37" width="10.7109375" customWidth="1"/>
+    <col min="38" max="38" width="10.7109375" customWidth="1"/>
+    <col min="39" max="39" width="10.7109375" customWidth="1"/>
+    <col min="40" max="40" width="10.7109375" customWidth="1"/>
+    <col min="41" max="41" width="10.7109375" customWidth="1"/>
+    <col min="42" max="42" width="10.7109375" customWidth="1"/>
+    <col min="43" max="43" width="10.7109375" customWidth="1"/>
+    <col min="44" max="44" width="10.7109375" customWidth="1"/>
+    <col min="45" max="45" width="10.7109375" customWidth="1"/>
+    <col min="46" max="46" width="10.7109375" customWidth="1"/>
+    <col min="47" max="47" width="10.7109375" customWidth="1"/>
+    <col min="48" max="48" width="10.7109375" customWidth="1"/>
+    <col min="49" max="49" width="10.7109375" customWidth="1"/>
+    <col min="50" max="50" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="27" customHeight="1">
@@ -900,7 +903,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="15">
-        <v>67.96899999999999</v>
+        <v>67.968</v>
       </c>
       <c r="C4" s="15">
         <v>69.16200000000001</v>
@@ -964,29 +967,29 @@
       <c r="AX4" s="4"/>
     </row>
     <row r="5" spans="1:50" ht="27" customHeight="1">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="18">
-        <v>56.617</v>
+      <c r="B5" s="15">
+        <v>62.095</v>
       </c>
-      <c r="C5" s="18">
-        <v>60.952</v>
+      <c r="C5" s="15">
+        <v>65.012</v>
       </c>
-      <c r="D5" s="18">
-        <v>0.235827</v>
+      <c r="D5" s="15">
+        <v>0.133103</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="13" t="str">
         <f> -D5/D12+1</f>
-        <v>0.387397</v>
+        <v>0.772646</v>
       </c>
-      <c r="H5" s="20" t="str">
+      <c r="H5" s="16" t="str">
         <f>C5/C12 -1</f>
-        <v>-0.027925</v>
+        <v>-0.006009</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="4"/>
@@ -1032,15 +1035,31 @@
       <c r="AX5" s="4"/>
     </row>
     <row r="6" spans="1:50" ht="27" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="A6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="18">
+        <v>56.617</v>
+      </c>
+      <c r="C6" s="18">
+        <v>60.952</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.235827</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="13" t="str">
+        <f> -D6/D13+1</f>
+        <v>0.387397</v>
+      </c>
+      <c r="H6" s="20" t="str">
+        <f>C6/C13 -1</f>
+        <v>-0.027925</v>
+      </c>
+      <c r="I6" s="9"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
@@ -1137,7 +1156,7 @@
     </row>
     <row r="8" spans="1:50" ht="27" customHeight="1">
       <c r="A8" s="21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -1211,7 +1230,7 @@
         <v>6</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -1270,7 +1289,7 @@
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G10" s="25" t="str">
         <f> -G3</f>
@@ -1325,7 +1344,7 @@
     </row>
     <row r="11" spans="1:50" ht="27" customHeight="1">
       <c r="A11" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="11">
         <v>68.03700000000001</v>
@@ -1338,7 +1357,7 @@
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="14" t="str">
+      <c r="G11" s="9" t="str">
         <f> -G4</f>
         <v>-0.805187</v>
       </c>
@@ -1390,27 +1409,27 @@
       <c r="AX11" s="4"/>
     </row>
     <row r="12" spans="1:50" ht="27" customHeight="1">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="28">
-        <v>57.711</v>
+      <c r="B12" s="4">
+        <v>62.854</v>
       </c>
-      <c r="C12" s="28">
-        <v>62.703</v>
+      <c r="C12" s="4">
+        <v>65.405</v>
       </c>
-      <c r="D12" s="28">
-        <v>0.384959</v>
+      <c r="D12" s="4">
+        <v>0.585444</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="17" t="str">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="9" t="str">
         <f> -G5</f>
-        <v>-0.387397</v>
+        <v>-0.772646</v>
       </c>
       <c r="H12" s="13" t="str">
         <f> -H5</f>
-        <v>0.027925</v>
+        <v>0.006009</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="4"/>
@@ -1456,15 +1475,29 @@
       <c r="AX12" s="4"/>
     </row>
     <row r="13" spans="1:50" ht="27" customHeight="1">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="A13" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="28">
+        <v>57.711</v>
+      </c>
+      <c r="C13" s="28">
+        <v>62.703</v>
+      </c>
+      <c r="D13" s="28">
+        <v>0.384959</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="9" t="str">
+        <f> -G6</f>
+        <v>-0.387397</v>
+      </c>
+      <c r="H13" s="13" t="str">
+        <f> -H6</f>
+        <v>0.027925</v>
+      </c>
+      <c r="I13" s="9"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -3432,23 +3465,25 @@
       <c r="AX50" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="I2:I6"/>
+    <mergeCell ref="I2:I6"/>
+    <mergeCell ref="I2:I6"/>
+    <mergeCell ref="I2:I6"/>
+    <mergeCell ref="I2:I6"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A8:D8"/>
-    <mergeCell ref="I9:I12"/>
-    <mergeCell ref="I9:I12"/>
-    <mergeCell ref="I9:I12"/>
-    <mergeCell ref="I9:I12"/>
+    <mergeCell ref="I9:I13"/>
+    <mergeCell ref="I9:I13"/>
+    <mergeCell ref="I9:I13"/>
+    <mergeCell ref="I9:I13"/>
+    <mergeCell ref="I9:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3462,56 +3497,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" customWidth="1"/>
-    <col min="23" max="23" width="10.85546875" customWidth="1"/>
-    <col min="24" max="24" width="10.85546875" customWidth="1"/>
-    <col min="25" max="25" width="10.85546875" customWidth="1"/>
-    <col min="26" max="26" width="10.85546875" customWidth="1"/>
-    <col min="27" max="27" width="10.85546875" customWidth="1"/>
-    <col min="28" max="28" width="10.85546875" customWidth="1"/>
-    <col min="29" max="29" width="10.85546875" customWidth="1"/>
-    <col min="30" max="30" width="10.85546875" customWidth="1"/>
-    <col min="31" max="31" width="10.85546875" customWidth="1"/>
-    <col min="32" max="32" width="10.85546875" customWidth="1"/>
-    <col min="33" max="33" width="10.85546875" customWidth="1"/>
-    <col min="34" max="34" width="10.85546875" customWidth="1"/>
-    <col min="35" max="35" width="10.85546875" customWidth="1"/>
-    <col min="36" max="36" width="10.85546875" customWidth="1"/>
-    <col min="37" max="37" width="10.85546875" customWidth="1"/>
-    <col min="38" max="38" width="10.85546875" customWidth="1"/>
-    <col min="39" max="39" width="10.85546875" customWidth="1"/>
-    <col min="40" max="40" width="10.85546875" customWidth="1"/>
-    <col min="41" max="41" width="10.85546875" customWidth="1"/>
-    <col min="42" max="42" width="10.85546875" customWidth="1"/>
-    <col min="43" max="43" width="10.85546875" customWidth="1"/>
-    <col min="44" max="44" width="10.85546875" customWidth="1"/>
-    <col min="45" max="45" width="10.85546875" customWidth="1"/>
-    <col min="46" max="46" width="10.85546875" customWidth="1"/>
-    <col min="47" max="47" width="10.85546875" customWidth="1"/>
-    <col min="48" max="48" width="10.85546875" customWidth="1"/>
-    <col min="49" max="49" width="10.85546875" customWidth="1"/>
-    <col min="50" max="50" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" customWidth="1"/>
+    <col min="23" max="23" width="10.7109375" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" customWidth="1"/>
+    <col min="27" max="27" width="10.7109375" customWidth="1"/>
+    <col min="28" max="28" width="10.7109375" customWidth="1"/>
+    <col min="29" max="29" width="10.7109375" customWidth="1"/>
+    <col min="30" max="30" width="10.7109375" customWidth="1"/>
+    <col min="31" max="31" width="10.7109375" customWidth="1"/>
+    <col min="32" max="32" width="10.7109375" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" customWidth="1"/>
+    <col min="34" max="34" width="10.7109375" customWidth="1"/>
+    <col min="35" max="35" width="10.7109375" customWidth="1"/>
+    <col min="36" max="36" width="10.7109375" customWidth="1"/>
+    <col min="37" max="37" width="10.7109375" customWidth="1"/>
+    <col min="38" max="38" width="10.7109375" customWidth="1"/>
+    <col min="39" max="39" width="10.7109375" customWidth="1"/>
+    <col min="40" max="40" width="10.7109375" customWidth="1"/>
+    <col min="41" max="41" width="10.7109375" customWidth="1"/>
+    <col min="42" max="42" width="10.7109375" customWidth="1"/>
+    <col min="43" max="43" width="10.7109375" customWidth="1"/>
+    <col min="44" max="44" width="10.7109375" customWidth="1"/>
+    <col min="45" max="45" width="10.7109375" customWidth="1"/>
+    <col min="46" max="46" width="10.7109375" customWidth="1"/>
+    <col min="47" max="47" width="10.7109375" customWidth="1"/>
+    <col min="48" max="48" width="10.7109375" customWidth="1"/>
+    <col min="49" max="49" width="10.7109375" customWidth="1"/>
+    <col min="50" max="50" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="27" customHeight="1">
@@ -6127,56 +6162,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" customWidth="1"/>
-    <col min="23" max="23" width="10.85546875" customWidth="1"/>
-    <col min="24" max="24" width="10.85546875" customWidth="1"/>
-    <col min="25" max="25" width="10.85546875" customWidth="1"/>
-    <col min="26" max="26" width="10.85546875" customWidth="1"/>
-    <col min="27" max="27" width="10.85546875" customWidth="1"/>
-    <col min="28" max="28" width="10.85546875" customWidth="1"/>
-    <col min="29" max="29" width="10.85546875" customWidth="1"/>
-    <col min="30" max="30" width="10.85546875" customWidth="1"/>
-    <col min="31" max="31" width="10.85546875" customWidth="1"/>
-    <col min="32" max="32" width="10.85546875" customWidth="1"/>
-    <col min="33" max="33" width="10.85546875" customWidth="1"/>
-    <col min="34" max="34" width="10.85546875" customWidth="1"/>
-    <col min="35" max="35" width="10.85546875" customWidth="1"/>
-    <col min="36" max="36" width="10.85546875" customWidth="1"/>
-    <col min="37" max="37" width="10.85546875" customWidth="1"/>
-    <col min="38" max="38" width="10.85546875" customWidth="1"/>
-    <col min="39" max="39" width="10.85546875" customWidth="1"/>
-    <col min="40" max="40" width="10.85546875" customWidth="1"/>
-    <col min="41" max="41" width="10.85546875" customWidth="1"/>
-    <col min="42" max="42" width="10.85546875" customWidth="1"/>
-    <col min="43" max="43" width="10.85546875" customWidth="1"/>
-    <col min="44" max="44" width="10.85546875" customWidth="1"/>
-    <col min="45" max="45" width="10.85546875" customWidth="1"/>
-    <col min="46" max="46" width="10.85546875" customWidth="1"/>
-    <col min="47" max="47" width="10.85546875" customWidth="1"/>
-    <col min="48" max="48" width="10.85546875" customWidth="1"/>
-    <col min="49" max="49" width="10.85546875" customWidth="1"/>
-    <col min="50" max="50" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" customWidth="1"/>
+    <col min="23" max="23" width="10.7109375" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" customWidth="1"/>
+    <col min="27" max="27" width="10.7109375" customWidth="1"/>
+    <col min="28" max="28" width="10.7109375" customWidth="1"/>
+    <col min="29" max="29" width="10.7109375" customWidth="1"/>
+    <col min="30" max="30" width="10.7109375" customWidth="1"/>
+    <col min="31" max="31" width="10.7109375" customWidth="1"/>
+    <col min="32" max="32" width="10.7109375" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" customWidth="1"/>
+    <col min="34" max="34" width="10.7109375" customWidth="1"/>
+    <col min="35" max="35" width="10.7109375" customWidth="1"/>
+    <col min="36" max="36" width="10.7109375" customWidth="1"/>
+    <col min="37" max="37" width="10.7109375" customWidth="1"/>
+    <col min="38" max="38" width="10.7109375" customWidth="1"/>
+    <col min="39" max="39" width="10.7109375" customWidth="1"/>
+    <col min="40" max="40" width="10.7109375" customWidth="1"/>
+    <col min="41" max="41" width="10.7109375" customWidth="1"/>
+    <col min="42" max="42" width="10.7109375" customWidth="1"/>
+    <col min="43" max="43" width="10.7109375" customWidth="1"/>
+    <col min="44" max="44" width="10.7109375" customWidth="1"/>
+    <col min="45" max="45" width="10.7109375" customWidth="1"/>
+    <col min="46" max="46" width="10.7109375" customWidth="1"/>
+    <col min="47" max="47" width="10.7109375" customWidth="1"/>
+    <col min="48" max="48" width="10.7109375" customWidth="1"/>
+    <col min="49" max="49" width="10.7109375" customWidth="1"/>
+    <col min="50" max="50" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="27" customHeight="1">

</xml_diff>